<commit_message>
edit export excel and fixing status column => still cannot render properly
</commit_message>
<xml_diff>
--- a/public/Report.xlsx
+++ b/public/Report.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,39 @@
   </si>
   <si>
     <t>SubName</t>
+  </si>
+  <si>
+    <t>20200313</t>
+  </si>
+  <si>
+    <t>999999</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>20150531</t>
+  </si>
+  <si>
+    <t>20160531</t>
+  </si>
+  <si>
+    <t>undefined</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Akiyama</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Training/Support</t>
   </si>
   <si>
     <t>Time Sheet</t>
@@ -931,7 +964,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="D2" sqref="D2"/>
@@ -1007,153 +1040,53 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>8</v>
-      </c>
-      <c r="E2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2">
+        <v>180</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2">
         <v>10</v>
       </c>
-      <c r="F2">
-        <v>12</v>
-      </c>
-      <c r="G2">
-        <v>14</v>
-      </c>
-      <c r="H2">
-        <v>16</v>
-      </c>
-      <c r="I2">
-        <v>18</v>
-      </c>
       <c r="J2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="K2">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L2">
+        <v>30</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
         <v>24</v>
       </c>
-      <c r="M2">
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
         <v>26</v>
-      </c>
-      <c r="N2">
-        <v>28</v>
-      </c>
-      <c r="O2">
-        <v>30</v>
-      </c>
-      <c r="P2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>15</v>
-      </c>
-      <c r="F3">
-        <v>18</v>
-      </c>
-      <c r="G3">
-        <v>21</v>
-      </c>
-      <c r="H3">
-        <v>24</v>
-      </c>
-      <c r="I3">
-        <v>27</v>
-      </c>
-      <c r="J3">
-        <v>30</v>
-      </c>
-      <c r="K3">
-        <v>33</v>
-      </c>
-      <c r="L3">
-        <v>36</v>
-      </c>
-      <c r="M3">
-        <v>39</v>
-      </c>
-      <c r="N3">
-        <v>42</v>
-      </c>
-      <c r="O3">
-        <v>45</v>
-      </c>
-      <c r="P3">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>16</v>
-      </c>
-      <c r="E4">
-        <v>20</v>
-      </c>
-      <c r="F4">
-        <v>24</v>
-      </c>
-      <c r="G4">
-        <v>28</v>
-      </c>
-      <c r="H4">
-        <v>32</v>
-      </c>
-      <c r="I4">
-        <v>36</v>
-      </c>
-      <c r="J4">
-        <v>40</v>
-      </c>
-      <c r="K4">
-        <v>44</v>
-      </c>
-      <c r="L4">
-        <v>48</v>
-      </c>
-      <c r="M4">
-        <v>52</v>
-      </c>
-      <c r="N4">
-        <v>56</v>
-      </c>
-      <c r="O4">
-        <v>60</v>
-      </c>
-      <c r="P4">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1180,7 +1113,7 @@
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1208,7 +1141,7 @@
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>13</v>
@@ -1218,16 +1151,16 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="5" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="L3" s="10"/>
     </row>
@@ -1242,18 +1175,18 @@
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="14" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" ht="26.25" customHeight="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="7"/>
@@ -1307,7 +1240,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="I7" s="24" t="s">
         <v>7</v>
@@ -1318,7 +1251,7 @@
     </row>
     <row r="8" ht="15.75" customHeight="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C8" s="27">
         <v>25599.625</v>
@@ -1337,7 +1270,7 @@
     </row>
     <row r="9" ht="15.75" customHeight="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="24" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
@@ -1385,7 +1318,7 @@
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="G1" s="38">
         <v>43896</v>
@@ -1405,18 +1338,18 @@
     </row>
     <row r="2" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -1425,7 +1358,7 @@
         <v>43896</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -1434,7 +1367,7 @@
         <v>43897</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -1443,7 +1376,7 @@
         <v>43898</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -1452,7 +1385,7 @@
         <v>43899</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -1461,7 +1394,7 @@
         <v>43900</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
@@ -1470,7 +1403,7 @@
         <v>43901</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
@@ -1479,35 +1412,35 @@
         <v>43902</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>